<commit_message>
Two additions to blog list
</commit_message>
<xml_diff>
--- a/content/posts/data/hello_world/list_of_blogs.xlsx
+++ b/content/posts/data/hello_world/list_of_blogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markd\Documents\GitHub\mark-druffel.com\content\posts\data\hello_world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4A0153-2F43-4256-B7B0-812C20E400A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0063E0-A707-4DC8-88E0-F205E9D4DC45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82E0AC8B-D962-4CC5-8D69-EE66D9834C91}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="282">
   <si>
     <t>URL</t>
   </si>
@@ -859,6 +859,24 @@
   </si>
   <si>
     <t>Python, Apache Superset, Apache Airflow</t>
+  </si>
+  <si>
+    <t>https://www.tylermw.com/</t>
+  </si>
+  <si>
+    <t>tylermorganwall</t>
+  </si>
+  <si>
+    <t>Tyler Morgan-Wall</t>
+  </si>
+  <si>
+    <t>https://www.fromthebottomoftheheap.net</t>
+  </si>
+  <si>
+    <t>Gavin Simpson</t>
+  </si>
+  <si>
+    <t>ucfagls</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E8684A-55A9-4DB5-9C0F-C20AF2B4BBB4}">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2703,6 +2721,34 @@
       </c>
       <c r="F84" s="1" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" t="s">
+        <v>277</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" t="s">
+        <v>281</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2789,6 +2835,8 @@
     <hyperlink ref="F82" r:id="rId80" xr:uid="{A3558910-0B28-4098-ABA3-573509CBC61E}"/>
     <hyperlink ref="F83" r:id="rId81" xr:uid="{44BFCD34-F6F8-4552-A3D2-A0BD9592FEA7}"/>
     <hyperlink ref="F84" r:id="rId82" xr:uid="{9E958094-D3C6-4776-B08C-3F1A87A1F5FE}"/>
+    <hyperlink ref="F85" r:id="rId83" xr:uid="{F8ABB5A2-B69D-4A21-BBF6-DADF98757B03}"/>
+    <hyperlink ref="F86" r:id="rId84" xr:uid="{F00E7630-4C89-47D1-98A7-188AFD4390D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>